<commit_message>
thêm thống kê tổng quát
</commit_message>
<xml_diff>
--- a/report/Laptopdb.xlsx
+++ b/report/Laptopdb.xlsx
@@ -638,7 +638,7 @@
         <v>15</v>
       </c>
       <c r="E2" t="n">
-        <v>100.0</v>
+        <v>16.0</v>
       </c>
       <c r="F2" t="n">
         <v>10250.0</v>
@@ -714,7 +714,7 @@
         <v>31</v>
       </c>
       <c r="E4" t="n">
-        <v>100.0</v>
+        <v>99.0</v>
       </c>
       <c r="F4" t="n">
         <v>1200.0</v>
@@ -752,7 +752,7 @@
         <v>39</v>
       </c>
       <c r="E5" t="n">
-        <v>100.0</v>
+        <v>99.0</v>
       </c>
       <c r="F5" t="n">
         <v>1000.0</v>
@@ -866,7 +866,7 @@
         <v>56</v>
       </c>
       <c r="E8" t="n">
-        <v>100.0</v>
+        <v>99.0</v>
       </c>
       <c r="F8" t="n">
         <v>9000.0</v>

</xml_diff>